<commit_message>
constants, jmxs, version tags
</commit_message>
<xml_diff>
--- a/dataHunterPerformanceTestSamples/mark59serverprofiles.xlsx
+++ b/dataHunterPerformanceTestSamples/mark59serverprofiles.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\temp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\gitrepo\mark-5-9\mark59-wip\dataHunterPerformanceTestSamples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9D2A9DF4-4E39-40EB-A26A-E97C1C754990}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFF4B554-EF74-49A1-AA5B-4418AB7A86B7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29685" yWindow="1605" windowWidth="27600" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="32325" yWindow="735" windowWidth="23250" windowHeight="12570" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SERVERPROFILES" sheetId="1" r:id="rId1"/>
@@ -24,11 +24,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="369" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="423" uniqueCount="145">
   <si>
     <t>SERVER_PROFILE_NAME</t>
   </si>
   <si>
+    <t>EXECUTOR</t>
+  </si>
+  <si>
     <t>SERVER</t>
   </si>
   <si>
@@ -44,9 +47,6 @@
     <t>PASSWORD_CIPHER</t>
   </si>
   <si>
-    <t>OPERATING_SYSTEM</t>
-  </si>
-  <si>
     <t>CONNECTION_PORT</t>
   </si>
   <si>
@@ -56,24 +56,30 @@
     <t>COMMENT</t>
   </si>
   <si>
+    <t>PARAMETERS</t>
+  </si>
+  <si>
     <t>DemoLINUX-DataHunterSeleniumDeployAndExecute</t>
   </si>
   <si>
+    <t>SSH_LINIX_UNIX</t>
+  </si>
+  <si>
     <t>localhost</t>
   </si>
   <si>
     <t/>
   </si>
   <si>
-    <t>LINUX</t>
-  </si>
-  <si>
     <t>22</t>
   </si>
   <si>
     <t>60000</t>
   </si>
   <si>
+    <t>{}</t>
+  </si>
+  <si>
     <t>DemoLINUX-DataHunterSeleniumGenJmeterReport</t>
   </si>
   <si>
@@ -89,7 +95,7 @@
     <t>DemoWIN-DataHunterSeleniumDeployAndExecute</t>
   </si>
   <si>
-    <t>WINDOWS</t>
+    <t>WMIC_WINDOWS</t>
   </si>
   <si>
     <t>DemoWIN-DataHunterSeleniumGenJmeterReport</t>
@@ -101,6 +107,27 @@
     <t>DemoWIN-DataHunterSeleniumRunCheck</t>
   </si>
   <si>
+    <t>NewRelicTestProfile</t>
+  </si>
+  <si>
+    <t>GROOVY_SCRIPT</t>
+  </si>
+  <si>
+    <t>supplied sample New Relic API groovy script</t>
+  </si>
+  <si>
+    <t>{"proxyPort":"","newRelicXapiKey":"","proxyServer":"","newRelicApiAppId":""}</t>
+  </si>
+  <si>
+    <t>SimpleScriptSampleRunner</t>
+  </si>
+  <si>
+    <t>runs a supplied, basic groovy script sample</t>
+  </si>
+  <si>
+    <t>{"parm1":"11","parm2":"55.7","parm3":"333"}</t>
+  </si>
+  <si>
     <t>localhost_LINUX</t>
   </si>
   <si>
@@ -134,15 +161,15 @@
     <t>UnixVMName</t>
   </si>
   <si>
-    <t>UNIX</t>
-  </si>
-  <si>
     <t>remoteWinServer</t>
   </si>
   <si>
     <t>WinServerName</t>
   </si>
   <si>
+    <t>xnr</t>
+  </si>
+  <si>
     <t>COMMAND_NAME</t>
   </si>
   <si>
@@ -164,6 +191,12 @@
     <t>DataHunterSeleniumRunCheck</t>
   </si>
   <si>
+    <t>NewRelicSampleCmd</t>
+  </si>
+  <si>
+    <t>SimpleScriptSampleCmd</t>
+  </si>
+  <si>
     <t>LINUX_free_m_1_1</t>
   </si>
   <si>
@@ -185,16 +218,13 @@
     <t>UNIX_lparstat_5_1</t>
   </si>
   <si>
-    <t>EXECUTOR</t>
-  </si>
-  <si>
     <t>COMMAND</t>
   </si>
   <si>
     <t>IGNORE_STDERR</t>
   </si>
   <si>
-    <t>WMIC_WINDOWS</t>
+    <t>PARAM_NAMES</t>
   </si>
   <si>
     <t xml:space="preserve">process call create 'cmd.exe /c 
@@ -230,7 +260,7 @@
     <t xml:space="preserve">refer DeployDataHunterTestArtifactsToJmeter.bat and DataHunterExecuteJmeterTest.bat in dataHunterPerformanceTestSamples </t>
   </si>
   <si>
-    <t>SSH_LINIX_UNIX</t>
+    <t>[]</t>
   </si>
   <si>
     <t>echo This script runs the JMeter deploy in the background, then opens a terminal for JMeter execution.
@@ -314,6 +344,116 @@
   </si>
   <si>
     <t>mpstat 1 1</t>
+  </si>
+  <si>
+    <t>import java.net.HttpURLConnection;
+import java.net.InetSocketAddress;
+import java.net.Proxy;
+import java.net.URL;
+import java.time.ZoneOffset;
+import java.time.ZonedDateTime;
+import java.time.format.DateTimeFormatter;
+import java.util.ArrayList;
+import java.util.List;
+import java.util.Scanner;
+import org.apache.commons.lang3.StringUtils;
+import org.json.JSONArray;
+import org.json.JSONObject;
+import com.mark59.servermetricsweb.pojos.ParsedMetric;
+import com.mark59.servermetricsweb.pojos.ScriptResponse;
+ScriptResponse scriptResponse = new ScriptResponse(); 
+List&lt;ParsedMetric&gt; parsedMetrics = new ArrayList&lt;ParsedMetric&gt;();
+String newRelicApiUrl = "https://api.newrelic.com/v2/applications/";
+String url = newRelicApiUrl + newRelicApiAppId + "/instances.json"; 
+String debugJsonResponses =  "running profile " + serverProfile.serverProfileName + ", init req : " + url ;
+JSONObject jsonResponse = null;
+Proxy proxy = StringUtils.isNotBlank(proxyServer + proxyPort) ? new Proxy(Proxy.Type.HTTP, new InetSocketAddress(proxyServer , new Integer(proxyPort))) : null;
+try {
+	HttpURLConnection conn = proxy != null ? (HttpURLConnection)new URL(url).openConnection(proxy) : (HttpURLConnection)new URL(url).openConnection();
+	conn.setRequestMethod("GET");
+	conn.addRequestProperty("X-Api-Key", newRelicXapiKey);
+	conn.setRequestProperty("Content-Type", "application/json");
+	conn.setRequestProperty("Accept", "application/json");
+	if (conn.getResponseCode() != HttpURLConnection.HTTP_OK) {
+		throw new Exception("rc:" + conn.getResponseCode() + "from " + url);
+	}
+	String isStr = null;
+	Scanner s = new Scanner(conn.getInputStream());
+	isStr = s.hasNext() ? s.next() : "";
+	jsonResponse = new JSONObject(isStr);
+	debugJsonResponses =  debugJsonResponses + "&lt;br&gt;init res.: " + jsonResponse.toString();
+	ZonedDateTime utcTimeNow = ZonedDateTime.now(ZoneOffset.UTC);
+	String toHour 	= String.format("%02d", utcTimeNow.getHour());
+	String toMinute	= String.format("%02d", utcTimeNow.getMinute());
+	ZonedDateTime utcMinus1Min = utcTimeNow.minusMinutes(1);
+	String fromHour	= String.format("%02d", utcMinus1Min.getHour());
+	String fromMinute = String.format("%02d", utcMinus1Min.getMinute());
+	String fromDate = utcMinus1Min.format(DateTimeFormatter.ofPattern("yyyy-MM-dd"));
+	String toDate 	= utcTimeNow.format(DateTimeFormatter.ofPattern("yyyy-MM-dd"));		
+	String urlDateRangeParmStr = "&amp;from=" + fromDate + "T" + fromHour + "%3A" + fromMinute + "%3A00%2B00%3A00" + "&amp;to=" + toDate + "T" + toHour + "%3A" + toMinute + "%3A00%2B00%3A00";
+	JSONArray application_instances = jsonResponse.getJSONArray("application_instances");
+	for (int i = 0; i &lt; application_instances.length(); i++) {
+		JSONObject application_instance = (JSONObject) application_instances.get(i);
+		Integer instanceId = (Integer) application_instance.get("id");
+		String instanceName = ((String)application_instance.get("application_name")).replace(":","_");
+		url = newRelicApiUrl + newRelicApiAppId  + "/instances/" + instanceId + "/metrics/data.json?names%5B%5D=Memory%2FHeap%2FFree&amp;names%5B%5D=CPU%2FUser%2FUtilization" + urlDateRangeParmStr;
+		debugJsonResponses =  debugJsonResponses + "&lt;br&gt;&lt;br&gt;req." + i + ": " + url ; 
+		conn = proxy != null ? (HttpURLConnection)new URL(url).openConnection(proxy) : (HttpURLConnection)new URL(url).openConnection();
+		conn.setRequestMethod("GET");
+		conn. addRequestProperty("X-Api-Key", newRelicXapiKey);
+		conn.setRequestProperty("Content-Type", "application/json");
+		conn.setRequestProperty("Accept", "application/json");
+		if (conn.getResponseCode() != HttpURLConnection.HTTP_OK) {
+			throw new Exception("rc:" + conn.getResponseCode() + "from " + url);
+		}
+		isStr = null;
+		s = new Scanner(conn.getInputStream());
+		isStr = s.hasNext() ? s.next() : "";
+		jsonResponse = new JSONObject(isStr);
+		debugJsonResponses =  debugJsonResponses + "&lt;br&gt;res." + i + ": " + jsonResponse.toString(); 
+		Number totalUusedMbMemory = -1.0;
+		totalUusedMbMemory =  (Number)((JSONObject)((JSONObject)jsonResponse.getJSONObject("metric_data").getJSONArray("metrics").get(0)).getJSONArray("timeslices").get(0)).getJSONObject("values").get("total_used_mb") ;
+		parsedMetrics.add(new ParsedMetric("MEMORY_" + newRelicApiAppId + "_" + instanceId + "_" + instanceName, totalUusedMbMemory,  "MEMORY"));
+		Number percentCpuUserUtilization = -1.0;
+		percentCpuUserUtilization = (Number)((JSONObject)((JSONObject)jsonResponse.getJSONObject("metric_data").getJSONArray("metrics").get(1)).getJSONArray("timeslices").get(0)).getJSONObject("values").get("percent");
+		parsedMetrics.add(new ParsedMetric("CPU_" + newRelicApiAppId + "_" + instanceId + "_" + instanceName, percentCpuUserUtilization, "CPU_UTIL"));
+	}
+} catch (Exception e) {
+	debugJsonResponses =  debugJsonResponses + "&lt;br&gt;\n ERROR :  Exception last url: " + url + ", response of  : " + jsonResponse + ", message: "+ e.getMessage(); 
+}
+scriptResponse.setCommandLog(debugJsonResponses);
+scriptResponse.setParsedMetrics(parsedMetrics);
+return scriptResponse;</t>
+  </si>
+  <si>
+    <t>NewRelic Supplied Sample</t>
+  </si>
+  <si>
+    <t>["newRelicApiAppId","newRelicXapiKey","proxyServer","proxyPort"]</t>
+  </si>
+  <si>
+    <t>import java.util.ArrayList;
+import java.util.List;
+import com.mark59.servermetricsweb.data.beans.ServerProfile;
+import com.mark59.servermetricsweb.pojos.ParsedMetric;
+import com.mark59.servermetricsweb.pojos.ScriptResponse;
+ScriptResponse scriptResponse = new ScriptResponse();
+List&lt;ParsedMetric&gt; parsedMetrics = new ArrayList&lt;ParsedMetric&gt;();
+String commandLogDebug = "running script " + serverProfile.getServerProfileName() + "&lt;br&gt;" +  serverProfile.getComment();
+commandLogDebug += "&lt;br&gt;passed parms : parm1=" + parm1 + ", parm2=" + parm2 + ", parm3=" + parm3
+Number aNumber = 123;
+parsedMetrics.add(new ParsedMetric("a_memory_txn", aNumber, "MEMORY"));
+parsedMetrics.add(new ParsedMetric("a_cpu_util_txn", 33.3,  "CPU_UTIL"));
+parsedMetrics.add(new ParsedMetric("some_datapoint", 66.6,  "DATAPOINT"));
+scriptResponse.setCommandLog(commandLogDebug);
+scriptResponse.setParsedMetrics(parsedMetrics);
+return scriptResponse;</t>
+  </si>
+  <si>
+    <t>supplied basic groovy script sample</t>
+  </si>
+  <si>
+    <t>["parm1","parm2","parm3"]</t>
   </si>
   <si>
     <t>vmstat=$(vmstat -v); 
@@ -962,25 +1102,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J13"/>
+  <dimension ref="A1:K15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="48.21875" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.77734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.77734375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.77734375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.44140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.77734375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.44140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="19.5546875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="23.21875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="102.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="152.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1011,389 +1154,456 @@
       <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I2" t="s">
+        <v>16</v>
+      </c>
+      <c r="J2" t="s">
+        <v>14</v>
+      </c>
+      <c r="K2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" t="s">
         <v>12</v>
       </c>
-      <c r="D2" t="s">
+      <c r="C3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G3" t="s">
+        <v>14</v>
+      </c>
+      <c r="H3" t="s">
+        <v>15</v>
+      </c>
+      <c r="I3" t="s">
+        <v>16</v>
+      </c>
+      <c r="J3" t="s">
+        <v>19</v>
+      </c>
+      <c r="K3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" t="s">
         <v>12</v>
       </c>
-      <c r="E2" t="s">
+      <c r="C4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G4" t="s">
+        <v>14</v>
+      </c>
+      <c r="H4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I4" t="s">
+        <v>16</v>
+      </c>
+      <c r="J4" t="s">
+        <v>21</v>
+      </c>
+      <c r="K4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G5" t="s">
+        <v>14</v>
+      </c>
+      <c r="H5" t="s">
+        <v>14</v>
+      </c>
+      <c r="I5" t="s">
+        <v>14</v>
+      </c>
+      <c r="J5" t="s">
+        <v>14</v>
+      </c>
+      <c r="K5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E6" t="s">
+        <v>14</v>
+      </c>
+      <c r="F6" t="s">
+        <v>14</v>
+      </c>
+      <c r="G6" t="s">
+        <v>14</v>
+      </c>
+      <c r="H6" t="s">
+        <v>14</v>
+      </c>
+      <c r="I6" t="s">
+        <v>14</v>
+      </c>
+      <c r="J6" t="s">
+        <v>25</v>
+      </c>
+      <c r="K6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" t="s">
+        <v>14</v>
+      </c>
+      <c r="E7" t="s">
+        <v>14</v>
+      </c>
+      <c r="F7" t="s">
+        <v>14</v>
+      </c>
+      <c r="G7" t="s">
+        <v>14</v>
+      </c>
+      <c r="H7" t="s">
+        <v>14</v>
+      </c>
+      <c r="I7" t="s">
+        <v>14</v>
+      </c>
+      <c r="J7" t="s">
+        <v>21</v>
+      </c>
+      <c r="K7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>27</v>
+      </c>
+      <c r="B8" t="s">
+        <v>28</v>
+      </c>
+      <c r="J8" t="s">
+        <v>29</v>
+      </c>
+      <c r="K8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>31</v>
+      </c>
+      <c r="B9" t="s">
+        <v>28</v>
+      </c>
+      <c r="J9" t="s">
+        <v>32</v>
+      </c>
+      <c r="K9" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>34</v>
+      </c>
+      <c r="B10" t="s">
         <v>12</v>
       </c>
-      <c r="F2" t="s">
+      <c r="C10" t="s">
+        <v>13</v>
+      </c>
+      <c r="D10" t="s">
+        <v>14</v>
+      </c>
+      <c r="E10" t="s">
+        <v>14</v>
+      </c>
+      <c r="F10" t="s">
+        <v>14</v>
+      </c>
+      <c r="G10" t="s">
+        <v>14</v>
+      </c>
+      <c r="H10" t="s">
+        <v>15</v>
+      </c>
+      <c r="I10" t="s">
+        <v>16</v>
+      </c>
+      <c r="J10" t="s">
+        <v>14</v>
+      </c>
+      <c r="K10" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>35</v>
+      </c>
+      <c r="B11" t="s">
+        <v>23</v>
+      </c>
+      <c r="C11" t="s">
+        <v>13</v>
+      </c>
+      <c r="D11" t="s">
+        <v>14</v>
+      </c>
+      <c r="E11" t="s">
+        <v>14</v>
+      </c>
+      <c r="F11" t="s">
+        <v>14</v>
+      </c>
+      <c r="G11" t="s">
+        <v>14</v>
+      </c>
+      <c r="H11" t="s">
+        <v>14</v>
+      </c>
+      <c r="I11" t="s">
+        <v>14</v>
+      </c>
+      <c r="J11" t="s">
+        <v>14</v>
+      </c>
+      <c r="K11" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>36</v>
+      </c>
+      <c r="B12" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12" t="s">
+        <v>13</v>
+      </c>
+      <c r="D12" t="s">
+        <v>37</v>
+      </c>
+      <c r="E12" t="s">
+        <v>14</v>
+      </c>
+      <c r="F12" t="s">
+        <v>14</v>
+      </c>
+      <c r="G12" t="s">
+        <v>14</v>
+      </c>
+      <c r="H12" t="s">
+        <v>14</v>
+      </c>
+      <c r="I12" t="s">
+        <v>14</v>
+      </c>
+      <c r="J12" t="s">
+        <v>38</v>
+      </c>
+      <c r="K12" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>39</v>
+      </c>
+      <c r="B13" t="s">
         <v>12</v>
       </c>
-      <c r="G2" t="s">
-        <v>13</v>
-      </c>
-      <c r="H2" t="s">
-        <v>14</v>
-      </c>
-      <c r="I2" t="s">
+      <c r="C13" t="s">
+        <v>40</v>
+      </c>
+      <c r="D13" t="s">
+        <v>14</v>
+      </c>
+      <c r="E13" t="s">
+        <v>41</v>
+      </c>
+      <c r="F13" t="s">
+        <v>42</v>
+      </c>
+      <c r="G13" t="s">
+        <v>14</v>
+      </c>
+      <c r="H13" t="s">
         <v>15</v>
       </c>
-      <c r="J2" t="s">
+      <c r="I13" t="s">
+        <v>16</v>
+      </c>
+      <c r="J13" t="s">
+        <v>14</v>
+      </c>
+      <c r="K13" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>43</v>
+      </c>
+      <c r="B14" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="C14" t="s">
+        <v>44</v>
+      </c>
+      <c r="D14" t="s">
+        <v>14</v>
+      </c>
+      <c r="E14" t="s">
+        <v>41</v>
+      </c>
+      <c r="F14" t="s">
+        <v>42</v>
+      </c>
+      <c r="G14" t="s">
+        <v>14</v>
+      </c>
+      <c r="H14" t="s">
+        <v>15</v>
+      </c>
+      <c r="I14" t="s">
         <v>16</v>
       </c>
-      <c r="B3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E3" t="s">
-        <v>12</v>
-      </c>
-      <c r="F3" t="s">
-        <v>12</v>
-      </c>
-      <c r="G3" t="s">
-        <v>13</v>
-      </c>
-      <c r="H3" t="s">
-        <v>14</v>
-      </c>
-      <c r="I3" t="s">
-        <v>15</v>
-      </c>
-      <c r="J3" t="s">
+      <c r="J14" t="s">
+        <v>14</v>
+      </c>
+      <c r="K14" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" t="s">
-        <v>12</v>
-      </c>
-      <c r="E4" t="s">
-        <v>12</v>
-      </c>
-      <c r="F4" t="s">
-        <v>12</v>
-      </c>
-      <c r="G4" t="s">
-        <v>13</v>
-      </c>
-      <c r="H4" t="s">
-        <v>14</v>
-      </c>
-      <c r="I4" t="s">
-        <v>15</v>
-      </c>
-      <c r="J4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>20</v>
-      </c>
-      <c r="B5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E5" t="s">
-        <v>12</v>
-      </c>
-      <c r="F5" t="s">
-        <v>12</v>
-      </c>
-      <c r="G5" t="s">
-        <v>21</v>
-      </c>
-      <c r="H5" t="s">
-        <v>12</v>
-      </c>
-      <c r="I5" t="s">
-        <v>12</v>
-      </c>
-      <c r="J5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>22</v>
-      </c>
-      <c r="B6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6" t="s">
-        <v>12</v>
-      </c>
-      <c r="D6" t="s">
-        <v>12</v>
-      </c>
-      <c r="E6" t="s">
-        <v>12</v>
-      </c>
-      <c r="F6" t="s">
-        <v>12</v>
-      </c>
-      <c r="G6" t="s">
-        <v>21</v>
-      </c>
-      <c r="H6" t="s">
-        <v>12</v>
-      </c>
-      <c r="I6" t="s">
-        <v>12</v>
-      </c>
-      <c r="J6" t="s">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>45</v>
+      </c>
+      <c r="B15" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>24</v>
-      </c>
-      <c r="B7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7" t="s">
-        <v>12</v>
-      </c>
-      <c r="D7" t="s">
-        <v>12</v>
-      </c>
-      <c r="E7" t="s">
-        <v>12</v>
-      </c>
-      <c r="F7" t="s">
-        <v>12</v>
-      </c>
-      <c r="G7" t="s">
-        <v>21</v>
-      </c>
-      <c r="H7" t="s">
-        <v>12</v>
-      </c>
-      <c r="I7" t="s">
-        <v>12</v>
-      </c>
-      <c r="J7" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>25</v>
-      </c>
-      <c r="B8" t="s">
-        <v>11</v>
-      </c>
-      <c r="C8" t="s">
-        <v>12</v>
-      </c>
-      <c r="D8" t="s">
-        <v>12</v>
-      </c>
-      <c r="E8" t="s">
-        <v>12</v>
-      </c>
-      <c r="F8" t="s">
-        <v>12</v>
-      </c>
-      <c r="G8" t="s">
-        <v>13</v>
-      </c>
-      <c r="H8" t="s">
-        <v>14</v>
-      </c>
-      <c r="I8" t="s">
-        <v>15</v>
-      </c>
-      <c r="J8" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>26</v>
-      </c>
-      <c r="B9" t="s">
-        <v>11</v>
-      </c>
-      <c r="C9" t="s">
-        <v>12</v>
-      </c>
-      <c r="D9" t="s">
-        <v>12</v>
-      </c>
-      <c r="E9" t="s">
-        <v>12</v>
-      </c>
-      <c r="F9" t="s">
-        <v>12</v>
-      </c>
-      <c r="G9" t="s">
-        <v>21</v>
-      </c>
-      <c r="H9" t="s">
-        <v>12</v>
-      </c>
-      <c r="I9" t="s">
-        <v>12</v>
-      </c>
-      <c r="J9" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>27</v>
-      </c>
-      <c r="B10" t="s">
-        <v>11</v>
-      </c>
-      <c r="C10" t="s">
-        <v>28</v>
-      </c>
-      <c r="D10" t="s">
-        <v>12</v>
-      </c>
-      <c r="E10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F10" t="s">
-        <v>12</v>
-      </c>
-      <c r="G10" t="s">
-        <v>21</v>
-      </c>
-      <c r="H10" t="s">
-        <v>12</v>
-      </c>
-      <c r="I10" t="s">
-        <v>12</v>
-      </c>
-      <c r="J10" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>30</v>
-      </c>
-      <c r="B11" t="s">
-        <v>31</v>
-      </c>
-      <c r="C11" t="s">
-        <v>12</v>
-      </c>
-      <c r="D11" t="s">
-        <v>32</v>
-      </c>
-      <c r="E11" t="s">
-        <v>33</v>
-      </c>
-      <c r="F11" t="s">
-        <v>12</v>
-      </c>
-      <c r="G11" t="s">
-        <v>13</v>
-      </c>
-      <c r="H11" t="s">
-        <v>14</v>
-      </c>
-      <c r="I11" t="s">
-        <v>15</v>
-      </c>
-      <c r="J11" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>34</v>
-      </c>
-      <c r="B12" t="s">
-        <v>35</v>
-      </c>
-      <c r="C12" t="s">
-        <v>12</v>
-      </c>
-      <c r="D12" t="s">
-        <v>32</v>
-      </c>
-      <c r="E12" t="s">
-        <v>33</v>
-      </c>
-      <c r="F12" t="s">
-        <v>12</v>
-      </c>
-      <c r="G12" t="s">
-        <v>36</v>
-      </c>
-      <c r="H12" t="s">
-        <v>14</v>
-      </c>
-      <c r="I12" t="s">
-        <v>15</v>
-      </c>
-      <c r="J12" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>37</v>
-      </c>
-      <c r="B13" t="s">
-        <v>38</v>
-      </c>
-      <c r="C13" t="s">
-        <v>12</v>
-      </c>
-      <c r="D13" t="s">
-        <v>32</v>
-      </c>
-      <c r="E13" t="s">
-        <v>33</v>
-      </c>
-      <c r="F13" t="s">
-        <v>12</v>
-      </c>
-      <c r="G13" t="s">
-        <v>21</v>
-      </c>
-      <c r="H13" t="s">
-        <v>12</v>
-      </c>
-      <c r="I13" t="s">
-        <v>12</v>
-      </c>
-      <c r="J13" t="s">
-        <v>12</v>
+      <c r="C15" t="s">
+        <v>46</v>
+      </c>
+      <c r="D15" t="s">
+        <v>14</v>
+      </c>
+      <c r="E15" t="s">
+        <v>41</v>
+      </c>
+      <c r="F15" t="s">
+        <v>42</v>
+      </c>
+      <c r="G15" t="s">
+        <v>14</v>
+      </c>
+      <c r="H15" t="s">
+        <v>14</v>
+      </c>
+      <c r="I15" t="s">
+        <v>14</v>
+      </c>
+      <c r="J15" t="s">
+        <v>14</v>
+      </c>
+      <c r="K15" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -1403,7 +1613,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:B22"/>
+  <dimension ref="A1:B25"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1418,175 +1628,199 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B2" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B3" t="s">
-        <v>41</v>
+        <v>50</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B4" t="s">
-        <v>42</v>
+        <v>51</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B5" t="s">
-        <v>43</v>
+        <v>52</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B6" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B7" t="s">
-        <v>45</v>
+        <v>54</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B8" t="s">
-        <v>46</v>
+        <v>55</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="B9" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="B10" t="s">
-        <v>48</v>
+        <v>57</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="B11" t="s">
-        <v>49</v>
+        <v>58</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>26</v>
+        <v>35</v>
       </c>
       <c r="B12" t="s">
-        <v>50</v>
+        <v>59</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>27</v>
+        <v>35</v>
       </c>
       <c r="B13" t="s">
-        <v>48</v>
+        <v>60</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>27</v>
+        <v>35</v>
       </c>
       <c r="B14" t="s">
-        <v>49</v>
+        <v>61</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="B15" t="s">
-        <v>50</v>
+        <v>59</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="B16" t="s">
-        <v>46</v>
+        <v>60</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="B17" t="s">
-        <v>47</v>
+        <v>61</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="B18" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="B19" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="B20" t="s">
-        <v>48</v>
+        <v>62</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="B21" t="s">
-        <v>49</v>
+        <v>63</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="B22" t="s">
-        <v>50</v>
+        <v>59</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>45</v>
+      </c>
+      <c r="B23" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>45</v>
+      </c>
+      <c r="B24" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>47</v>
+      </c>
+      <c r="B25" t="s">
+        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -1596,7 +1830,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:E15"/>
+  <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1607,261 +1841,347 @@
     <col min="3" max="3" width="223.88671875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.44140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="117.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="62.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>53</v>
+        <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>54</v>
+        <v>64</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>55</v>
+        <v>65</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>43</v>
+        <v>52</v>
       </c>
       <c r="B2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" t="s">
+        <v>67</v>
+      </c>
+      <c r="D2" t="s">
+        <v>68</v>
+      </c>
+      <c r="E2" t="s">
+        <v>69</v>
+      </c>
+      <c r="F2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" t="s">
+        <v>71</v>
+      </c>
+      <c r="D3" t="s">
+        <v>72</v>
+      </c>
+      <c r="E3" t="s">
+        <v>73</v>
+      </c>
+      <c r="F3" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" t="s">
+        <v>74</v>
+      </c>
+      <c r="D4" t="s">
+        <v>68</v>
+      </c>
+      <c r="E4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F4" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" t="s">
+        <v>75</v>
+      </c>
+      <c r="D5" t="s">
+        <v>72</v>
+      </c>
+      <c r="E5" t="s">
+        <v>76</v>
+      </c>
+      <c r="F5" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>54</v>
+      </c>
+      <c r="B6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" t="s">
+        <v>77</v>
+      </c>
+      <c r="D6" t="s">
+        <v>68</v>
+      </c>
+      <c r="E6" t="s">
+        <v>14</v>
+      </c>
+      <c r="F6" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>51</v>
+      </c>
+      <c r="B7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" t="s">
+        <v>78</v>
+      </c>
+      <c r="D7" t="s">
+        <v>72</v>
+      </c>
+      <c r="E7" t="s">
+        <v>79</v>
+      </c>
+      <c r="F7" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>59</v>
+      </c>
+      <c r="B8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" t="s">
+        <v>80</v>
+      </c>
+      <c r="D8" t="s">
+        <v>68</v>
+      </c>
+      <c r="E8" t="s">
+        <v>14</v>
+      </c>
+      <c r="F8" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>60</v>
+      </c>
+      <c r="B9" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" t="s">
+        <v>81</v>
+      </c>
+      <c r="D9" t="s">
+        <v>68</v>
+      </c>
+      <c r="E9" t="s">
+        <v>14</v>
+      </c>
+      <c r="F9" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>57</v>
+      </c>
+      <c r="B10" t="s">
+        <v>12</v>
+      </c>
+      <c r="C10" t="s">
+        <v>82</v>
+      </c>
+      <c r="D10" t="s">
+        <v>68</v>
+      </c>
+      <c r="E10" t="s">
+        <v>83</v>
+      </c>
+      <c r="F10" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>58</v>
+      </c>
+      <c r="B11" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" t="s">
+        <v>84</v>
+      </c>
+      <c r="D11" t="s">
+        <v>68</v>
+      </c>
+      <c r="E11" t="s">
+        <v>14</v>
+      </c>
+      <c r="F11" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>55</v>
+      </c>
+      <c r="B12" t="s">
+        <v>28</v>
+      </c>
+      <c r="C12" t="s">
+        <v>85</v>
+      </c>
+      <c r="D12" t="s">
+        <v>68</v>
+      </c>
+      <c r="E12" t="s">
+        <v>86</v>
+      </c>
+      <c r="F12" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
         <v>56</v>
       </c>
-      <c r="C2" t="s">
-        <v>57</v>
-      </c>
-      <c r="D2" t="s">
-        <v>58</v>
-      </c>
-      <c r="E2" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>40</v>
-      </c>
-      <c r="B3" t="s">
-        <v>60</v>
-      </c>
-      <c r="C3" t="s">
+      <c r="B13" t="s">
+        <v>28</v>
+      </c>
+      <c r="C13" t="s">
+        <v>88</v>
+      </c>
+      <c r="D13" t="s">
+        <v>68</v>
+      </c>
+      <c r="E13" t="s">
+        <v>89</v>
+      </c>
+      <c r="F13" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>62</v>
+      </c>
+      <c r="B14" t="s">
+        <v>12</v>
+      </c>
+      <c r="C14" t="s">
+        <v>91</v>
+      </c>
+      <c r="D14" t="s">
+        <v>68</v>
+      </c>
+      <c r="E14" t="s">
+        <v>14</v>
+      </c>
+      <c r="F14" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>92</v>
+      </c>
+      <c r="B15" t="s">
+        <v>12</v>
+      </c>
+      <c r="C15" t="s">
+        <v>91</v>
+      </c>
+      <c r="D15" t="s">
+        <v>68</v>
+      </c>
+      <c r="E15" t="s">
+        <v>14</v>
+      </c>
+      <c r="F15" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>63</v>
+      </c>
+      <c r="B16" t="s">
+        <v>12</v>
+      </c>
+      <c r="C16" t="s">
+        <v>93</v>
+      </c>
+      <c r="D16" t="s">
+        <v>68</v>
+      </c>
+      <c r="E16" t="s">
+        <v>14</v>
+      </c>
+      <c r="F16" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
         <v>61</v>
       </c>
-      <c r="D3" t="s">
-        <v>62</v>
-      </c>
-      <c r="E3" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>44</v>
-      </c>
-      <c r="B4" t="s">
-        <v>56</v>
-      </c>
-      <c r="C4" t="s">
-        <v>64</v>
-      </c>
-      <c r="D4" t="s">
-        <v>58</v>
-      </c>
-      <c r="E4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>41</v>
-      </c>
-      <c r="B5" t="s">
-        <v>60</v>
-      </c>
-      <c r="C5" t="s">
-        <v>65</v>
-      </c>
-      <c r="D5" t="s">
-        <v>62</v>
-      </c>
-      <c r="E5" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>45</v>
-      </c>
-      <c r="B6" t="s">
-        <v>56</v>
-      </c>
-      <c r="C6" t="s">
-        <v>67</v>
-      </c>
-      <c r="D6" t="s">
-        <v>58</v>
-      </c>
-      <c r="E6" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>42</v>
-      </c>
-      <c r="B7" t="s">
-        <v>60</v>
-      </c>
-      <c r="C7" t="s">
+      <c r="B17" t="s">
+        <v>23</v>
+      </c>
+      <c r="C17" t="s">
+        <v>94</v>
+      </c>
+      <c r="D17" t="s">
         <v>68</v>
       </c>
-      <c r="D7" t="s">
-        <v>62</v>
-      </c>
-      <c r="E7" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>48</v>
-      </c>
-      <c r="B8" t="s">
-        <v>56</v>
-      </c>
-      <c r="C8" t="s">
+      <c r="E17" t="s">
+        <v>14</v>
+      </c>
+      <c r="F17" t="s">
         <v>70</v>
-      </c>
-      <c r="D8" t="s">
-        <v>58</v>
-      </c>
-      <c r="E8" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>49</v>
-      </c>
-      <c r="B9" t="s">
-        <v>56</v>
-      </c>
-      <c r="C9" t="s">
-        <v>71</v>
-      </c>
-      <c r="D9" t="s">
-        <v>58</v>
-      </c>
-      <c r="E9" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>46</v>
-      </c>
-      <c r="B10" t="s">
-        <v>60</v>
-      </c>
-      <c r="C10" t="s">
-        <v>72</v>
-      </c>
-      <c r="D10" t="s">
-        <v>58</v>
-      </c>
-      <c r="E10" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>47</v>
-      </c>
-      <c r="B11" t="s">
-        <v>60</v>
-      </c>
-      <c r="C11" t="s">
-        <v>74</v>
-      </c>
-      <c r="D11" t="s">
-        <v>58</v>
-      </c>
-      <c r="E11" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>51</v>
-      </c>
-      <c r="B12" t="s">
-        <v>60</v>
-      </c>
-      <c r="C12" t="s">
-        <v>75</v>
-      </c>
-      <c r="D12" t="s">
-        <v>58</v>
-      </c>
-      <c r="E12" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>76</v>
-      </c>
-      <c r="B13" t="s">
-        <v>60</v>
-      </c>
-      <c r="C13" t="s">
-        <v>75</v>
-      </c>
-      <c r="D13" t="s">
-        <v>58</v>
-      </c>
-      <c r="E13" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>52</v>
-      </c>
-      <c r="B14" t="s">
-        <v>60</v>
-      </c>
-      <c r="C14" t="s">
-        <v>77</v>
-      </c>
-      <c r="D14" t="s">
-        <v>58</v>
-      </c>
-      <c r="E14" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>50</v>
-      </c>
-      <c r="B15" t="s">
-        <v>56</v>
-      </c>
-      <c r="C15" t="s">
-        <v>78</v>
-      </c>
-      <c r="D15" t="s">
-        <v>58</v>
-      </c>
-      <c r="E15" t="s">
-        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -1883,170 +2203,170 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>79</v>
+        <v>95</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>43</v>
+        <v>52</v>
       </c>
       <c r="B2" t="s">
-        <v>80</v>
+        <v>96</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="B3" t="s">
-        <v>80</v>
+        <v>96</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="B4" t="s">
-        <v>80</v>
+        <v>96</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="B5" t="s">
-        <v>80</v>
+        <v>96</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>45</v>
+        <v>54</v>
       </c>
       <c r="B6" t="s">
-        <v>80</v>
+        <v>96</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="B7" t="s">
-        <v>80</v>
+        <v>96</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>48</v>
+        <v>59</v>
       </c>
       <c r="B8" t="s">
-        <v>81</v>
+        <v>97</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>49</v>
+        <v>60</v>
       </c>
       <c r="B9" t="s">
-        <v>82</v>
+        <v>98</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>46</v>
+        <v>57</v>
       </c>
       <c r="B10" t="s">
-        <v>83</v>
+        <v>99</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>46</v>
+        <v>57</v>
       </c>
       <c r="B11" t="s">
-        <v>84</v>
+        <v>100</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>46</v>
+        <v>57</v>
       </c>
       <c r="B12" t="s">
-        <v>85</v>
+        <v>101</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>47</v>
+        <v>58</v>
       </c>
       <c r="B13" t="s">
-        <v>86</v>
+        <v>102</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>51</v>
+        <v>62</v>
       </c>
       <c r="B14" t="s">
-        <v>87</v>
+        <v>103</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>51</v>
+        <v>62</v>
       </c>
       <c r="B15" t="s">
-        <v>88</v>
+        <v>104</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>51</v>
+        <v>62</v>
       </c>
       <c r="B16" t="s">
-        <v>89</v>
+        <v>105</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>76</v>
+        <v>92</v>
       </c>
       <c r="B17" t="s">
-        <v>87</v>
+        <v>103</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>76</v>
+        <v>92</v>
       </c>
       <c r="B18" t="s">
-        <v>88</v>
+        <v>104</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>76</v>
+        <v>92</v>
       </c>
       <c r="B19" t="s">
-        <v>89</v>
+        <v>105</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>52</v>
+        <v>63</v>
       </c>
       <c r="B20" t="s">
-        <v>86</v>
+        <v>102</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>50</v>
+        <v>61</v>
       </c>
       <c r="B21" t="s">
-        <v>90</v>
+        <v>106</v>
       </c>
     </row>
   </sheetData>
@@ -2072,262 +2392,262 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>79</v>
+        <v>95</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>91</v>
+        <v>107</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>92</v>
+        <v>108</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>93</v>
+        <v>109</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>9</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>94</v>
+        <v>110</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>83</v>
+        <v>99</v>
       </c>
       <c r="B2" t="s">
-        <v>95</v>
+        <v>111</v>
       </c>
       <c r="C2" t="s">
-        <v>96</v>
+        <v>112</v>
       </c>
       <c r="D2" t="s">
-        <v>97</v>
+        <v>113</v>
       </c>
       <c r="E2" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="F2" t="s">
-        <v>98</v>
+        <v>114</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>84</v>
+        <v>100</v>
       </c>
       <c r="B3" t="s">
-        <v>95</v>
+        <v>111</v>
       </c>
       <c r="C3" t="s">
-        <v>99</v>
+        <v>115</v>
       </c>
       <c r="D3" t="s">
-        <v>100</v>
+        <v>116</v>
       </c>
       <c r="E3" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="F3" t="s">
-        <v>101</v>
+        <v>117</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>85</v>
+        <v>101</v>
       </c>
       <c r="B4" t="s">
-        <v>95</v>
+        <v>111</v>
       </c>
       <c r="C4" t="s">
-        <v>102</v>
+        <v>118</v>
       </c>
       <c r="D4" t="s">
-        <v>103</v>
+        <v>119</v>
       </c>
       <c r="E4" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="F4" t="s">
-        <v>101</v>
+        <v>117</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>81</v>
+        <v>97</v>
       </c>
       <c r="B5" t="s">
-        <v>95</v>
+        <v>111</v>
       </c>
       <c r="C5" t="s">
-        <v>104</v>
+        <v>120</v>
       </c>
       <c r="D5" t="s">
-        <v>105</v>
+        <v>121</v>
       </c>
       <c r="E5" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="F5" t="s">
-        <v>106</v>
+        <v>122</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>82</v>
+        <v>98</v>
       </c>
       <c r="B6" t="s">
-        <v>95</v>
+        <v>111</v>
       </c>
       <c r="C6" t="s">
-        <v>107</v>
+        <v>123</v>
       </c>
       <c r="D6" t="s">
-        <v>105</v>
+        <v>121</v>
       </c>
       <c r="E6" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="F6" t="s">
-        <v>108</v>
+        <v>124</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>109</v>
+        <v>125</v>
       </c>
       <c r="B7" t="s">
-        <v>110</v>
+        <v>126</v>
       </c>
       <c r="C7" t="s">
-        <v>111</v>
+        <v>127</v>
       </c>
       <c r="D7" t="s">
-        <v>112</v>
+        <v>128</v>
       </c>
       <c r="E7" t="s">
-        <v>113</v>
+        <v>129</v>
       </c>
       <c r="F7" t="s">
-        <v>114</v>
+        <v>130</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>86</v>
+        <v>102</v>
       </c>
       <c r="B8" t="s">
-        <v>110</v>
+        <v>126</v>
       </c>
       <c r="C8" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D8" t="s">
-        <v>115</v>
+        <v>131</v>
       </c>
       <c r="E8" t="s">
-        <v>113</v>
+        <v>129</v>
       </c>
       <c r="F8" t="s">
-        <v>114</v>
+        <v>130</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>80</v>
+        <v>96</v>
       </c>
       <c r="B9" t="s">
-        <v>116</v>
+        <v>132</v>
       </c>
       <c r="C9" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D9" t="s">
-        <v>117</v>
+        <v>133</v>
       </c>
       <c r="E9" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="F9" t="s">
-        <v>118</v>
+        <v>134</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>87</v>
+        <v>103</v>
       </c>
       <c r="B10" t="s">
-        <v>95</v>
+        <v>111</v>
       </c>
       <c r="C10" t="s">
-        <v>119</v>
+        <v>135</v>
       </c>
       <c r="D10" t="s">
-        <v>120</v>
+        <v>136</v>
       </c>
       <c r="E10" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="F10" t="s">
-        <v>121</v>
+        <v>137</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>88</v>
+        <v>104</v>
       </c>
       <c r="B11" t="s">
-        <v>95</v>
+        <v>111</v>
       </c>
       <c r="C11" t="s">
-        <v>122</v>
+        <v>138</v>
       </c>
       <c r="D11" t="s">
-        <v>123</v>
+        <v>139</v>
       </c>
       <c r="E11" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="F11" t="s">
-        <v>121</v>
+        <v>137</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>89</v>
+        <v>105</v>
       </c>
       <c r="B12" t="s">
-        <v>95</v>
+        <v>111</v>
       </c>
       <c r="C12" t="s">
-        <v>124</v>
+        <v>140</v>
       </c>
       <c r="D12" t="s">
-        <v>125</v>
+        <v>141</v>
       </c>
       <c r="E12" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="F12" t="s">
-        <v>121</v>
+        <v>137</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>90</v>
+        <v>106</v>
       </c>
       <c r="B13" t="s">
-        <v>110</v>
+        <v>126</v>
       </c>
       <c r="C13" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D13" t="s">
-        <v>126</v>
+        <v>142</v>
       </c>
       <c r="E13" t="s">
-        <v>127</v>
+        <v>143</v>
       </c>
       <c r="F13" t="s">
-        <v>128</v>
+        <v>144</v>
       </c>
     </row>
   </sheetData>

</xml_diff>